<commit_message>
Corrected typos in Klippy and Printer state names
Also added copies of three Moonraker API documents of which understanding seems key to interpreting how this code uses the API.
</commit_message>
<xml_diff>
--- a/doc/source/development/dgus_project/Interpreting T5LCFG_272480.xlsx
+++ b/doc/source/development/dgus_project/Interpreting T5LCFG_272480.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36A58F8-9BB4-402B-B196-CE5E3295D2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A11A57-122A-48C8-A5D9-0EA9B620D0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,21 +14,11 @@
     <sheet name="Translation Lookup Tables" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="291">
   <si>
     <t>Hex Address</t>
   </si>
@@ -892,6 +882,27 @@
   </si>
   <si>
     <t>3f</t>
+  </si>
+  <si>
+    <t>T5UID1.CFG</t>
+  </si>
+  <si>
+    <t>Screens.ICL file number = 184</t>
+  </si>
+  <si>
+    <t>Serial Interface Baud Rate = 8400bps</t>
+  </si>
+  <si>
+    <t>Normal + Startup backlight brightness = 0%</t>
+  </si>
+  <si>
+    <t>Backlight wakeup time after standby = 0ms</t>
+  </si>
+  <si>
+    <t>Flash-Reset T5UID1.CFG</t>
+  </si>
+  <si>
+    <t>a5</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1880,6 +1891,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1904,17 +1921,52 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2275,6 +2327,172 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="121920" cy="2065020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>279109</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>503424</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>51068</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5021580" y="9819349"/>
+          <a:ext cx="6370824" cy="1661719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>129122</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65B269B2-8D67-D0F7-B509-887270AA628B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4998720" y="11567160"/>
+          <a:ext cx="5326380" cy="1881722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2804,10 +3022,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL49"/>
+  <dimension ref="A1:AL67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2819,7 +3037,7 @@
   <sheetData>
     <row r="1" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="176" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="B1" s="177"/>
       <c r="C1" s="177"/>
@@ -2925,53 +3143,53 @@
       <c r="A3" s="179" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="B3">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>31</v>
+      </c>
+      <c r="F3" s="194">
+        <v>0</v>
+      </c>
+      <c r="G3" s="194">
+        <v>0</v>
+      </c>
+      <c r="H3" s="225">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
         <v>28</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>44</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
       </c>
       <c r="AH3" s="200"/>
       <c r="AI3" s="193"/>
@@ -3050,7 +3268,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>244</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>29</v>
@@ -3062,31 +3280,35 @@
         <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>244</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="AH5" s="203"/>
       <c r="AI5" s="194"/>
       <c r="AJ5" s="194"/>
@@ -3257,43 +3479,43 @@
       </c>
       <c r="G11" s="188" t="str">
         <f>RIGHT(D3,1)</f>
-        <v>c</v>
+        <v>4</v>
       </c>
       <c r="H11" s="187" t="str">
         <f>LEFT(E3,1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" s="188" t="str">
         <f>RIGHT(E3,1)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J11" s="187" t="str">
         <f>LEFT(F3,1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K11" s="188" t="str">
         <f>RIGHT(F3,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="187" t="str">
         <f>LEFT(G3,1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M11" s="188" t="str">
         <f>RIGHT(G3,1)</f>
-        <v>f</v>
+        <v>0</v>
       </c>
       <c r="N11" s="187" t="str">
         <f>LEFT(H3,1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O11" s="188" t="str">
         <f>RIGHT(H3,1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" s="187" t="str">
         <f>LEFT(I3,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="188" t="str">
         <f>RIGHT(I3,1)</f>
@@ -3301,43 +3523,43 @@
       </c>
       <c r="R11" s="187" t="str">
         <f>LEFT(J3,1)</f>
-        <v>2</v>
+        <v>b</v>
       </c>
       <c r="S11" s="188" t="str">
         <f>RIGHT(J3,1)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T11" s="187" t="str">
         <f>LEFT(K3,1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U11" s="188" t="str">
         <f>RIGHT(K3,1)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="V11" s="187" t="str">
         <f>LEFT(L3,1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W11" s="188" t="str">
         <f>RIGHT(L3,1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X11" s="187" t="str">
         <f>LEFT(M3,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="188" t="str">
         <f>RIGHT(M3,1)</f>
-        <v>c</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="187" t="str">
         <f>LEFT(N3,1)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AA11" s="188" t="str">
         <f>RIGHT(N3,1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB11" s="187" t="str">
         <f>LEFT(O3,1)</f>
@@ -3345,7 +3567,7 @@
       </c>
       <c r="AC11" s="188" t="str">
         <f>RIGHT(O3,1)</f>
-        <v>a</v>
+        <v>0</v>
       </c>
       <c r="AD11" s="187" t="str">
         <f>LEFT(P3,1)</f>
@@ -3353,15 +3575,15 @@
       </c>
       <c r="AE11" s="188" t="str">
         <f>RIGHT(P3,1)</f>
-        <v>b</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="187" t="str">
         <f>LEFT(Q3,1)</f>
-        <v>b</v>
+        <v>0</v>
       </c>
       <c r="AG11" t="str">
         <f>RIGHT(Q3,1)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="203"/>
       <c r="AI11" s="194"/>
@@ -3529,11 +3751,11 @@
       </c>
       <c r="F13" s="189" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="190" t="str">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H13" s="189" t="str">
         <f t="shared" si="6"/>
@@ -3561,11 +3783,11 @@
       </c>
       <c r="N13" s="189" t="str">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="190" t="str">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P13" s="189" t="str">
         <f t="shared" si="14"/>
@@ -3577,11 +3799,11 @@
       </c>
       <c r="R13" s="189" t="str">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="S13" s="190" t="str">
         <f t="shared" si="17"/>
-        <v>e</v>
+        <v>0</v>
       </c>
       <c r="T13" s="189" t="str">
         <f t="shared" si="18"/>
@@ -3589,15 +3811,15 @@
       </c>
       <c r="U13" s="190" t="str">
         <f t="shared" si="19"/>
-        <v>b</v>
+        <v>0</v>
       </c>
       <c r="V13" s="189" t="str">
         <f t="shared" si="20"/>
-        <v>b</v>
+        <v>0</v>
       </c>
       <c r="W13" s="190" t="str">
         <f t="shared" si="21"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="X13" s="189" t="str">
         <f t="shared" si="22"/>
@@ -3609,7 +3831,7 @@
       </c>
       <c r="Z13" s="189" t="str">
         <f t="shared" si="24"/>
-        <v>f</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="190" t="str">
         <f t="shared" si="25"/>
@@ -3617,11 +3839,11 @@
       </c>
       <c r="AB13" s="189" t="str">
         <f t="shared" si="26"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="190" t="str">
         <f t="shared" si="27"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD13" s="189" t="s">
         <v>259</v>
@@ -4753,6 +4975,442 @@
       </c>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
+    </row>
+    <row r="50" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A51" s="176" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="4">
+        <v>8</v>
+      </c>
+      <c r="K52" s="4">
+        <v>9</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="179" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>54</v>
+      </c>
+      <c r="C53">
+        <v>35</v>
+      </c>
+      <c r="D53">
+        <v>44</v>
+      </c>
+      <c r="E53">
+        <v>31</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>28</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>44</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="179" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="179" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A63" s="176" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="4">
+        <v>8</v>
+      </c>
+      <c r="K64" s="4">
+        <v>9</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P64" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="179" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>54</v>
+      </c>
+      <c r="C65">
+        <v>35</v>
+      </c>
+      <c r="D65">
+        <v>44</v>
+      </c>
+      <c r="E65">
+        <v>31</v>
+      </c>
+      <c r="F65" s="194" t="s">
+        <v>274</v>
+      </c>
+      <c r="G65" s="194" t="s">
+        <v>290</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>44</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="179" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="179" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4843,30 +5501,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection sqref="A1:P62"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="6" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="3.77734375" hidden="1" customWidth="1"/>
-    <col min="9" max="12" width="3.77734375" style="5" hidden="1" customWidth="1"/>
-    <col min="13" max="15" width="3.77734375" hidden="1" customWidth="1"/>
+    <col min="3" max="6" width="8.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="1" customWidth="1"/>
+    <col min="8" max="8" width="3.77734375" customWidth="1"/>
+    <col min="9" max="12" width="3.77734375" style="5" customWidth="1"/>
+    <col min="13" max="15" width="3.77734375" customWidth="1"/>
     <col min="16" max="16" width="52" customWidth="1"/>
     <col min="17" max="17" width="3.109375" customWidth="1"/>
     <col min="18" max="18" width="40.33203125" customWidth="1"/>
     <col min="19" max="19" width="40.44140625" customWidth="1"/>
     <col min="20" max="20" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="87" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="87" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="207" t="s">
         <v>76</v>
       </c>
@@ -4901,8 +5559,11 @@
       <c r="U1" s="6" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>119</v>
       </c>
@@ -4936,7 +5597,7 @@
       <c r="O2" s="213"/>
       <c r="P2" s="183" t="str">
         <f>'T5L CFG - HEX'!A1</f>
-        <v>T5LCFG_272480K.CFG</v>
+        <v>Flash-Reset T5UID1.CFG</v>
       </c>
       <c r="R2" s="44" t="s">
         <v>265</v>
@@ -4945,8 +5606,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="215" t="s">
+    <row r="3" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="217" t="s">
         <v>118</v>
       </c>
       <c r="B3" s="130" t="s">
@@ -5008,8 +5669,8 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="216"/>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="218"/>
       <c r="B4" s="131" t="s">
         <v>2</v>
       </c>
@@ -5066,8 +5727,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="216"/>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="218"/>
       <c r="B5" s="131" t="s">
         <v>3</v>
       </c>
@@ -5077,15 +5738,15 @@
       </c>
       <c r="D5" s="119" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!G$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!G$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1100</v>
+        <v>0100</v>
       </c>
       <c r="E5" s="118">
         <f>VLOOKUP(C5,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="F5" s="119" t="str">
+      <c r="F5" s="119">
         <f>VLOOKUP(D5,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>c</v>
+        <v>4</v>
       </c>
       <c r="G5" s="120"/>
       <c r="H5" s="121" t="str">
@@ -5106,7 +5767,7 @@
       </c>
       <c r="L5" s="124" t="str">
         <f>MID($D5,1,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="125" t="str">
         <f>MID($D5,2,1)</f>
@@ -5124,26 +5785,26 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="216"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="218"/>
       <c r="B6" s="131" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="118" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!H$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!H$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0100</v>
+        <v>0011</v>
       </c>
       <c r="D6" s="119" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!I$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!I$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0011</v>
+        <v>0001</v>
       </c>
       <c r="E6" s="118">
         <f>VLOOKUP(C6,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="119">
         <f>VLOOKUP(D6,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="120"/>
       <c r="H6" s="121" t="str">
@@ -5152,15 +5813,15 @@
       </c>
       <c r="I6" s="122" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="122" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="123" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="124" t="str">
         <f>MID($D6,1,1)</f>
@@ -5172,7 +5833,7 @@
       </c>
       <c r="N6" s="125" t="str">
         <f>MID($D6,3,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="126" t="str">
         <f>MID($D6,4,1)</f>
@@ -5182,26 +5843,26 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="216"/>
+    <row r="7" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="218"/>
       <c r="B7" s="131" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="118" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!J$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!J$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="D7" s="119" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!K$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!K$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="E7" s="118">
         <f>VLOOKUP(C7,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7" s="119">
         <f>VLOOKUP(D7,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="120"/>
       <c r="H7" s="121" t="str">
@@ -5214,11 +5875,11 @@
       </c>
       <c r="J7" s="122" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="123" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="124" t="str">
         <f>MID($D7,1,1)</f>
@@ -5234,13 +5895,13 @@
       </c>
       <c r="O7" s="126" t="str">
         <f>MID($D7,4,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="114" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
         <v>144</v>
       </c>
@@ -5249,19 +5910,19 @@
       </c>
       <c r="C8" s="45" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!L$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!L$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0011</v>
-      </c>
-      <c r="D8" s="46">
+        <v>0000</v>
+      </c>
+      <c r="D8" s="46" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!M$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!M$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1111</v>
+        <v>0000</v>
       </c>
       <c r="E8" s="45">
         <f>VLOOKUP(C8,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>3</v>
-      </c>
-      <c r="F8" s="46" t="str">
+        <v>0</v>
+      </c>
+      <c r="F8" s="46">
         <f>VLOOKUP(D8,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>f</v>
+        <v>0</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="47" t="str">
@@ -5291,8 +5952,11 @@
       <c r="U8" s="44" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="44" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="52" t="s">
         <v>139</v>
       </c>
@@ -5331,8 +5995,11 @@
       <c r="U9" s="44" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V9" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="52" t="s">
         <v>138</v>
       </c>
@@ -5348,7 +6015,7 @@
       <c r="I10" s="48"/>
       <c r="J10" s="48" t="str">
         <f>MID($C8,3,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="49"/>
       <c r="L10" s="50"/>
@@ -5357,7 +6024,7 @@
       <c r="O10" s="51"/>
       <c r="P10" s="172" t="str">
         <f>VLOOKUP(CONCATENATE(B10," = ",J10),'Translation Lookup Tables'!$H$2:$I$18,2,FALSE)</f>
-        <v>22 File initialization variable space - Load</v>
+        <v>22 File initialization variable space - Do Not Load</v>
       </c>
       <c r="R10" s="44" t="s">
         <v>222</v>
@@ -5371,8 +6038,11 @@
       <c r="U10" s="44" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V10" s="44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
         <v>145</v>
       </c>
@@ -5389,7 +6059,7 @@
       <c r="J11" s="48"/>
       <c r="K11" s="49" t="str">
         <f>MID($C8,4,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="50"/>
       <c r="M11" s="51"/>
@@ -5397,7 +6067,7 @@
       <c r="O11" s="51"/>
       <c r="P11" s="172" t="str">
         <f>VLOOKUP(CONCATENATE(B11," = ",K11),'Translation Lookup Tables'!$H$2:$I$18,2,FALSE)</f>
-        <v>Variable automatic upload setting - ON</v>
+        <v>Variable automatic upload setting - OFF</v>
       </c>
       <c r="R11" s="44" t="s">
         <v>226</v>
@@ -5411,8 +6081,11 @@
       <c r="U11" s="44" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V11" s="44" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="52" t="s">
         <v>149</v>
       </c>
@@ -5430,14 +6103,14 @@
       <c r="K12" s="49"/>
       <c r="L12" s="50" t="str">
         <f>MID($D8,1,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="51"/>
       <c r="N12" s="51"/>
       <c r="O12" s="51"/>
       <c r="P12" s="172" t="str">
         <f>VLOOKUP(CONCATENATE(B12," = ",L12),'Translation Lookup Tables'!$H$2:$I$18,2,FALSE)</f>
-        <v>Touchscreen Audio Control - Open</v>
+        <v>Touchscreen Audio Control - Close</v>
       </c>
       <c r="R12" s="44" t="s">
         <v>227</v>
@@ -5451,8 +6124,11 @@
       <c r="U12" s="44" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V12" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="60" t="s">
         <v>150</v>
       </c>
@@ -5471,13 +6147,13 @@
       <c r="L13" s="22"/>
       <c r="M13" s="23" t="str">
         <f>MID($D8,2,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="172" t="str">
         <f>VLOOKUP(CONCATENATE(B13," = ",M13),'Translation Lookup Tables'!$H$2:$I$18,2,FALSE)</f>
-        <v>Touchscreen Backlight Standby Control - Open</v>
+        <v>Touchscreen Backlight Standby Control - Close</v>
       </c>
       <c r="R13" s="44" t="s">
         <v>231</v>
@@ -5491,8 +6167,11 @@
       <c r="U13" s="44" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V13" s="44" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="76" t="s">
         <v>151</v>
       </c>
@@ -5512,15 +6191,15 @@
       <c r="M14" s="51"/>
       <c r="N14" s="51" t="str">
         <f>MID($D8,3,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="51" t="str">
         <f>MID($D8,4,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="173" t="str">
         <f>VLOOKUP(CONCATENATE(B14," = ",CONCATENATE(N14,O14)),'Translation Lookup Tables'!$H$2:$I$18,2,FALSE)</f>
-        <v>Orient Display to 270 degrees</v>
+        <v>Orient Display to 0 degrees</v>
       </c>
       <c r="R14" s="44" t="s">
         <v>238</v>
@@ -5534,8 +6213,11 @@
       <c r="U14" s="44" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="44" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="62" t="s">
         <v>129</v>
       </c>
@@ -5544,19 +6226,19 @@
       </c>
       <c r="C15" s="9" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!N$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!N$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="D15" s="21" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!O$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!O$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="E15" s="9">
         <f>VLOOKUP(C15,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="21">
         <f>VLOOKUP(D15,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="33"/>
       <c r="H15" s="41" t="str">
@@ -5586,8 +6268,11 @@
       <c r="U15" s="44" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V15" s="44" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="59" t="s">
         <v>131</v>
       </c>
@@ -5626,8 +6311,11 @@
       <c r="U16" s="44" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V16" s="44" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="59" t="s">
         <v>141</v>
       </c>
@@ -5643,7 +6331,7 @@
       <c r="I17" s="48"/>
       <c r="J17" s="48" t="str">
         <f>MID($C15,3,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="49"/>
       <c r="L17" s="50"/>
@@ -5652,7 +6340,7 @@
       <c r="O17" s="51"/>
       <c r="P17" s="172" t="str">
         <f>VLOOKUP(CONCATENATE(B17," = ",J17),'Translation Lookup Tables'!$H$2:$I$26,2,FALSE)</f>
-        <v>Do not reset SPI NAND Flash</v>
+        <v>RESET SPI NAND Flash, once (erases all data)</v>
       </c>
       <c r="R17" t="s">
         <v>252</v>
@@ -5666,8 +6354,11 @@
       <c r="U17" s="44" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V17" s="44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="59" t="s">
         <v>137</v>
       </c>
@@ -5706,8 +6397,11 @@
       <c r="U18" s="44" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V18" s="44" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78" t="s">
         <v>142</v>
       </c>
@@ -5733,7 +6427,7 @@
       </c>
       <c r="N19" s="73" t="str">
         <f>MID($D15,3,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="74" t="str">
         <f>MID($D15,4,1)</f>
@@ -5745,8 +6439,11 @@
       <c r="U19" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="103" t="s">
         <v>120</v>
       </c>
@@ -5755,7 +6452,7 @@
       </c>
       <c r="C20" s="105" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!P$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!P$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="D20" s="106" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!Q$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!Q$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
@@ -5763,7 +6460,7 @@
       </c>
       <c r="E20" s="105">
         <f>VLOOKUP(C20,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="106">
         <f>VLOOKUP(D20,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
@@ -5784,7 +6481,7 @@
       </c>
       <c r="K20" s="110" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="111" t="str">
         <f t="shared" ref="L20:L45" si="4">MID($D20,1,1)</f>
@@ -5804,7 +6501,7 @@
       </c>
       <c r="P20" s="114"/>
     </row>
-    <row r="21" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="56" t="s">
         <v>123</v>
       </c>
@@ -5813,24 +6510,24 @@
       </c>
       <c r="C21" s="45" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!R$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!R$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0010</v>
+        <v>1011</v>
       </c>
       <c r="D21" s="46" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!S$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!S$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0000</v>
-      </c>
-      <c r="E21" s="45">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="45" t="str">
         <f>VLOOKUP(C21,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>2</v>
+        <v>b</v>
       </c>
       <c r="F21" s="46">
         <f>VLOOKUP(D21,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G21" s="34"/>
       <c r="H21" s="47" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="48" t="str">
         <f t="shared" si="1"/>
@@ -5842,11 +6539,11 @@
       </c>
       <c r="K21" s="49" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="50" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="51" t="str">
         <f t="shared" si="5"/>
@@ -5862,7 +6559,7 @@
       </c>
       <c r="P21" s="148" t="str">
         <f>CONCATENATE("Screens.ICL file number = ",VLOOKUP('T5L CFG - Interpretation'!E21,'Translation Lookup Tables'!C3:D19,2,FALSE)*16+VLOOKUP('T5L CFG - Interpretation'!F21,'Translation Lookup Tables'!C3:D19,2,FALSE))</f>
-        <v>Screens.ICL file number = 32</v>
+        <v>Screens.ICL file number = 184</v>
       </c>
       <c r="R21" t="s">
         <v>262</v>
@@ -5876,8 +6573,11 @@
       <c r="U21" s="44" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V21" s="44" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="147" t="s">
         <v>121</v>
       </c>
@@ -5886,19 +6586,19 @@
       </c>
       <c r="C22" s="20" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!T$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!T$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="D22" s="20" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!U$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!U$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="E22" s="20">
         <f>VLOOKUP(C22,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22" s="20">
         <f>VLOOKUP(D22,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G22" s="30"/>
       <c r="H22" s="25" t="str">
@@ -5911,7 +6611,7 @@
       </c>
       <c r="J22" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="27" t="str">
         <f t="shared" si="3"/>
@@ -5919,7 +6619,7 @@
       </c>
       <c r="L22" s="25" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="26" t="str">
         <f t="shared" si="5"/>
@@ -5933,9 +6633,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P22" s="147" t="str">
+      <c r="P22" s="147" t="e">
         <f>CONCATENATE("Touchscreen reporting point rate = ",400/(VLOOKUP(E22,'Translation Lookup Tables'!C4:D19,2,FALSE)*16+VLOOKUP('T5L CFG - Interpretation'!F22,'Translation Lookup Tables'!C4:D19,2,FALSE)),"Hz")</f>
-        <v>Touchscreen reporting point rate = 10Hz</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="R22" t="s">
         <v>264</v>
@@ -5949,9 +6649,12 @@
       <c r="U22" s="44" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="217" t="s">
+      <c r="V22" s="44" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="219" t="s">
         <v>122</v>
       </c>
       <c r="B23" s="54" t="s">
@@ -5959,19 +6662,19 @@
       </c>
       <c r="C23" s="39" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!V$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!V$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="D23" s="40" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!W$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!W$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="E23" s="39">
         <f>VLOOKUP(C23,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F23" s="40">
         <f>VLOOKUP(D23,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="10" t="str">
@@ -5980,7 +6683,7 @@
       </c>
       <c r="I23" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="11" t="str">
         <f t="shared" si="2"/>
@@ -5996,7 +6699,7 @@
       </c>
       <c r="M23" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="23" t="str">
         <f t="shared" si="6"/>
@@ -6008,7 +6711,7 @@
       </c>
       <c r="P23" s="139" t="str">
         <f>CONCATENATE("Serial Interface Baud Rate = ",3225600/(VLOOKUP(E23,'Translation Lookup Tables'!C4:D19,2,FALSE)*64+VLOOKUP('T5L CFG - Interpretation'!F23,'Translation Lookup Tables'!C4:D19,2,FALSE)*32+VLOOKUP('T5L CFG - Interpretation'!E24,'Translation Lookup Tables'!C4:D19,2,FALSE)*16+VLOOKUP('T5L CFG - Interpretation'!F24,'Translation Lookup Tables'!C4:D19,2,FALSE)),"bps")</f>
-        <v>Serial Interface Baud Rate = 115200bps</v>
+        <v>Serial Interface Baud Rate = 8400bps</v>
       </c>
       <c r="R23" t="s">
         <v>269</v>
@@ -6022,27 +6725,30 @@
       <c r="U23" s="44" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="218"/>
+      <c r="V23" s="44" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="220"/>
       <c r="B24" s="55" t="s">
         <v>68</v>
       </c>
       <c r="C24" s="9" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!X$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!X$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="D24" s="21" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!Y$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!Y$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1100</v>
+        <v>0000</v>
       </c>
       <c r="E24" s="9">
         <f>VLOOKUP(C24,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="F24" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="F24" s="21">
         <f>VLOOKUP(D24,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>c</v>
+        <v>0</v>
       </c>
       <c r="G24" s="33"/>
       <c r="H24" s="41" t="str">
@@ -6059,15 +6765,15 @@
       </c>
       <c r="K24" s="17" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="28" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="42" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="42" t="str">
         <f t="shared" si="6"/>
@@ -6079,7 +6785,7 @@
       </c>
       <c r="P24" s="140"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
         <v>124</v>
       </c>
@@ -6088,19 +6794,19 @@
       </c>
       <c r="C25" s="8" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!Z$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!Z$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="D25" s="20" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AA$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AA$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="E25" s="8">
         <f>VLOOKUP(C25,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F25" s="20">
         <f>VLOOKUP(D25,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="13" t="str">
@@ -6109,11 +6815,11 @@
       </c>
       <c r="I25" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="15" t="str">
         <f t="shared" si="3"/>
@@ -6125,7 +6831,7 @@
       </c>
       <c r="M25" s="26" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" s="26" t="str">
         <f t="shared" si="6"/>
@@ -6137,7 +6843,7 @@
       </c>
       <c r="P25" t="str">
         <f>CONCATENATE("Normal + Startup backlight brightness = ",'T5L CFG - Interpretation'!E25*16+'T5L CFG - Interpretation'!F25,"%")</f>
-        <v>Normal + Startup backlight brightness = 100%</v>
+        <v>Normal + Startup backlight brightness = 0%</v>
       </c>
       <c r="R25" t="s">
         <v>257</v>
@@ -6151,8 +6857,11 @@
       <c r="U25" s="44" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V25" s="44" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44" t="s">
         <v>125</v>
       </c>
@@ -6165,15 +6874,15 @@
       </c>
       <c r="D26" s="20" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AC$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AC$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1010</v>
+        <v>0000</v>
       </c>
       <c r="E26" s="8">
         <f>VLOOKUP(C26,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="20" t="str">
+      <c r="F26" s="20">
         <f>VLOOKUP(D26,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>a</v>
+        <v>0</v>
       </c>
       <c r="G26" s="32"/>
       <c r="H26" s="13" t="str">
@@ -6194,7 +6903,7 @@
       </c>
       <c r="L26" s="25" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="26" t="str">
         <f t="shared" si="5"/>
@@ -6202,7 +6911,7 @@
       </c>
       <c r="N26" s="26" t="str">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="27" t="str">
         <f t="shared" si="7"/>
@@ -6210,7 +6919,7 @@
       </c>
       <c r="P26" t="str">
         <f>CONCATENATE("Standby backlight brightness = ",'T5L CFG - Interpretation'!E26*16+VLOOKUP('T5L CFG - Interpretation'!F26,'Translation Lookup Tables'!$C$3:$D$19,2,FALSE),"%")</f>
-        <v>Standby backlight brightness = 10%</v>
+        <v>Standby backlight brightness = 0%</v>
       </c>
       <c r="R26" t="s">
         <v>258</v>
@@ -6224,9 +6933,12 @@
       <c r="U26" s="44" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="219" t="s">
+      <c r="V26" s="44" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="221" t="s">
         <v>126</v>
       </c>
       <c r="B27" s="36" t="s">
@@ -6238,15 +6950,15 @@
       </c>
       <c r="D27" s="40" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AE$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AE$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1011</v>
+        <v>0000</v>
       </c>
       <c r="E27" s="39">
         <f>VLOOKUP(C27,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="40" t="str">
+      <c r="F27" s="40">
         <f>VLOOKUP(D27,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>b</v>
+        <v>0</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="10" t="str">
@@ -6267,7 +6979,7 @@
       </c>
       <c r="L27" s="22" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="23" t="str">
         <f t="shared" si="5"/>
@@ -6275,15 +6987,15 @@
       </c>
       <c r="N27" s="23" t="str">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27" t="str">
         <f>CONCATENATE("Backlight wakeup time after standby = ",(VLOOKUP(E27,'Translation Lookup Tables'!C4:D19,2,FALSE)*64+VLOOKUP('T5L CFG - Interpretation'!F27,'Translation Lookup Tables'!C4:D19,2,FALSE)*32+VLOOKUP('T5L CFG - Interpretation'!E28,'Translation Lookup Tables'!C4:D19,2,FALSE)*16+VLOOKUP('T5L CFG - Interpretation'!F28,'Translation Lookup Tables'!C4:D19,2,FALSE))*10,"ms")</f>
-        <v>Backlight wakeup time after standby = 5360ms</v>
+        <v>Backlight wakeup time after standby = 0ms</v>
       </c>
       <c r="R27" t="s">
         <v>267</v>
@@ -6297,32 +7009,35 @@
       <c r="U27" s="44" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="220"/>
+      <c r="V27" s="44" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="222"/>
       <c r="B28" s="38" t="s">
         <v>72</v>
       </c>
       <c r="C28" s="9" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AF$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AF$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1011</v>
+        <v>0000</v>
       </c>
       <c r="D28" s="21" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AG$11),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AG$11,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1000</v>
-      </c>
-      <c r="E28" s="9" t="str">
+        <v>0000</v>
+      </c>
+      <c r="E28" s="9">
         <f>VLOOKUP(C28,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>b</v>
+        <v>0</v>
       </c>
       <c r="F28" s="21">
         <f>VLOOKUP(D28,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G28" s="33"/>
       <c r="H28" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="16" t="str">
         <f t="shared" si="1"/>
@@ -6330,15 +7045,15 @@
       </c>
       <c r="J28" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="17" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="28" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="42" t="str">
         <f t="shared" si="5"/>
@@ -6355,9 +7070,12 @@
       <c r="P28" s="184" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="221" t="s">
+      <c r="V28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="223" t="s">
         <v>158</v>
       </c>
       <c r="B29" s="81" t="s">
@@ -6415,9 +7133,12 @@
       <c r="P29" s="91" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="222"/>
+      <c r="V29" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="224"/>
       <c r="B30" s="92" t="s">
         <v>91</v>
       </c>
@@ -6473,8 +7194,11 @@
       <c r="P30" s="102" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="103" t="s">
         <v>200</v>
       </c>
@@ -6532,7 +7256,7 @@
       </c>
       <c r="P31" s="114"/>
     </row>
-    <row r="32" spans="1:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="103" t="s">
         <v>201</v>
       </c>
@@ -6590,7 +7314,7 @@
       </c>
       <c r="P32" s="114"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="115" t="s">
         <v>202</v>
       </c>
@@ -6648,7 +7372,7 @@
       </c>
       <c r="P33" s="114"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="116" t="s">
         <v>203</v>
       </c>
@@ -6706,8 +7430,8 @@
       </c>
       <c r="P34" s="114"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="223" t="s">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="215" t="s">
         <v>204</v>
       </c>
       <c r="B35" s="117" t="s">
@@ -6762,10 +7486,10 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P35" s="224"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="223"/>
+      <c r="P35" s="216"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="215"/>
       <c r="B36" s="117" t="s">
         <v>97</v>
       </c>
@@ -6818,9 +7542,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P36" s="224"/>
-    </row>
-    <row r="37" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P36" s="216"/>
+    </row>
+    <row r="37" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="127" t="s">
         <v>205</v>
       </c>
@@ -6878,7 +7602,7 @@
       </c>
       <c r="P37" s="114"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="116" t="s">
         <v>206</v>
       </c>
@@ -6936,7 +7660,7 @@
       </c>
       <c r="P38" s="114"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="116" t="s">
         <v>207</v>
       </c>
@@ -6994,8 +7718,8 @@
       </c>
       <c r="P39" s="114"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="223" t="s">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="215" t="s">
         <v>208</v>
       </c>
       <c r="B40" s="117" t="s">
@@ -7050,10 +7774,10 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P40" s="224"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="223"/>
+      <c r="P40" s="216"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="215"/>
       <c r="B41" s="117" t="s">
         <v>102</v>
       </c>
@@ -7106,9 +7830,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P41" s="224"/>
-    </row>
-    <row r="42" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P41" s="216"/>
+    </row>
+    <row r="42" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="116" t="s">
         <v>209</v>
       </c>
@@ -7166,7 +7890,7 @@
       </c>
       <c r="P42" s="114"/>
     </row>
-    <row r="43" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="128" t="s">
         <v>159</v>
       </c>
@@ -7225,8 +7949,11 @@
       <c r="P43" s="91" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="64" t="s">
         <v>161</v>
       </c>
@@ -7285,8 +8012,11 @@
       <c r="P44" s="75" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V44" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="134" t="s">
         <v>163</v>
       </c>
@@ -7345,8 +8075,11 @@
       <c r="P45" s="91" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="115" t="s">
         <v>166</v>
       </c>
@@ -7393,8 +8126,11 @@
       <c r="P46" s="143" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="116" t="s">
         <v>174</v>
       </c>
@@ -7420,8 +8156,11 @@
       <c r="P47" s="145" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V47" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="116" t="s">
         <v>175</v>
       </c>
@@ -7447,8 +8186,11 @@
       <c r="P48" s="145" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V48" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="116" t="s">
         <v>177</v>
       </c>
@@ -7474,8 +8216,11 @@
       <c r="P49" s="145" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="127" t="s">
         <v>179</v>
       </c>
@@ -7501,8 +8246,11 @@
       <c r="P50" s="136" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V50" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="128" t="s">
         <v>181</v>
       </c>
@@ -7511,7 +8259,7 @@
       </c>
       <c r="C51" s="105" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!F$13),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!F$13,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="D51" s="106" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!G$12),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!G$12,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
@@ -7519,7 +8267,7 @@
       </c>
       <c r="E51" s="105">
         <f>VLOOKUP(C51,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" s="106">
         <f>VLOOKUP(D51,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
@@ -7540,7 +8288,7 @@
       </c>
       <c r="K51" s="110" t="str">
         <f t="shared" ref="K51:K62" si="15">MID($C51,4,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" s="111" t="str">
         <f t="shared" ref="L51:L62" si="16">MID($D51,1,1)</f>
@@ -7561,8 +8309,11 @@
       <c r="P51" s="146" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V51" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="103" t="s">
         <v>183</v>
       </c>
@@ -7621,8 +8372,11 @@
       <c r="P52" s="137" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="132" t="s">
         <v>185</v>
       </c>
@@ -7681,8 +8435,11 @@
       <c r="P53" s="133" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V53" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="103" t="s">
         <v>186</v>
       </c>
@@ -7741,8 +8498,11 @@
       <c r="P54" s="107" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="103" t="s">
         <v>187</v>
       </c>
@@ -7751,7 +8511,7 @@
       </c>
       <c r="C55" s="105" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!N$13),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!N$13,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="D55" s="106" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!O$12),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!O$12,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
@@ -7759,7 +8519,7 @@
       </c>
       <c r="E55" s="105">
         <f>VLOOKUP(C55,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="106">
         <f>VLOOKUP(D55,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
@@ -7780,7 +8540,7 @@
       </c>
       <c r="K55" s="110" t="str">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" s="111" t="str">
         <f t="shared" si="16"/>
@@ -7801,8 +8561,11 @@
       <c r="P55" s="107" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="V55" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="134" t="s">
         <v>189</v>
       </c>
@@ -7861,8 +8624,11 @@
       <c r="P56" s="135" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="116" t="s">
         <v>191</v>
       </c>
@@ -7871,7 +8637,7 @@
       </c>
       <c r="C57" s="118" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!R$13),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!R$13,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="D57" s="119" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!S$12),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!S$12,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
@@ -7879,7 +8645,7 @@
       </c>
       <c r="E57" s="118">
         <f>VLOOKUP(C57,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F57" s="119">
         <f>VLOOKUP(D57,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
@@ -7892,11 +8658,11 @@
       </c>
       <c r="I57" s="122" t="str">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" s="122" t="str">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" s="123" t="str">
         <f t="shared" si="15"/>
@@ -7921,8 +8687,11 @@
       <c r="P57" s="120" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="V57" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="115" t="s">
         <v>192</v>
       </c>
@@ -7981,23 +8750,26 @@
       <c r="P58" s="84" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="127"/>
       <c r="B59" s="92" t="s">
         <v>114</v>
       </c>
       <c r="C59" s="93" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!V$13),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!V$13,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1011</v>
+        <v>0000</v>
       </c>
       <c r="D59" s="94" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!W$12),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!W$12,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
         <v>0000</v>
       </c>
-      <c r="E59" s="93" t="str">
+      <c r="E59" s="93">
         <f>VLOOKUP(C59,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>b</v>
+        <v>0</v>
       </c>
       <c r="F59" s="94">
         <f>VLOOKUP(D59,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
@@ -8006,7 +8778,7 @@
       <c r="G59" s="95"/>
       <c r="H59" s="96" t="str">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" s="97" t="str">
         <f t="shared" si="13"/>
@@ -8014,11 +8786,11 @@
       </c>
       <c r="J59" s="97" t="str">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K59" s="98" t="str">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59" s="99" t="str">
         <f t="shared" si="16"/>
@@ -8038,7 +8810,7 @@
       </c>
       <c r="P59" s="136"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="115" t="s">
         <v>194</v>
       </c>
@@ -8097,23 +8869,26 @@
       <c r="P60" s="84" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="127"/>
       <c r="B61" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="93">
+      <c r="C61" s="93" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!Z$13),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!Z$13,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>1111</v>
+        <v>0000</v>
       </c>
       <c r="D61" s="94" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AA$12),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AA$12,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
         <v>0000</v>
       </c>
-      <c r="E61" s="93" t="str">
+      <c r="E61" s="93">
         <f>VLOOKUP(C61,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>f</v>
+        <v>0</v>
       </c>
       <c r="F61" s="94">
         <f>VLOOKUP(D61,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
@@ -8122,19 +8897,19 @@
       <c r="G61" s="95"/>
       <c r="H61" s="96" t="str">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="97" t="str">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" s="97" t="str">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61" s="98" t="str">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" s="99" t="str">
         <f t="shared" si="16"/>
@@ -8154,7 +8929,7 @@
       </c>
       <c r="P61" s="136"/>
     </row>
-    <row r="62" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="103" t="s">
         <v>196</v>
       </c>
@@ -8163,7 +8938,7 @@
       </c>
       <c r="C62" s="105" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AB$13),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AB$13,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="D62" s="106" t="str">
         <f>IFERROR(VLOOKUP(VALUE('T5L CFG - HEX'!AC$12),'Translation Lookup Tables'!$A$3:$B$19,2,FALSE),VLOOKUP('T5L CFG - HEX'!AC$12,'Translation Lookup Tables'!$A$3:$B$19,2,FALSE))</f>
@@ -8171,7 +8946,7 @@
       </c>
       <c r="E62" s="105">
         <f>VLOOKUP(C62,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F62" s="106">
         <f>VLOOKUP(D62,'Translation Lookup Tables'!$B$3:$C$19,2,FALSE)</f>
@@ -8184,11 +8959,11 @@
       </c>
       <c r="I62" s="109" t="str">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" s="109" t="str">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" s="110" t="str">
         <f t="shared" si="15"/>
@@ -8213,8 +8988,11 @@
       <c r="P62" s="137" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="V62" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63"/>
@@ -8224,7 +9002,7 @@
       <c r="K63"/>
       <c r="L63"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C64"/>
       <c r="D64"/>
       <c r="E64"/>
@@ -8252,62 +9030,78 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="S25:T26">
-    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>$R25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" stopIfTrue="1" operator="equal">
       <formula>$R25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S21:U21">
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="notEqual">
+  <conditionalFormatting sqref="S21:V21">
+    <cfRule type="cellIs" dxfId="19" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>$R21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" stopIfTrue="1" operator="equal">
       <formula>$R21</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S22:U22">
-    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="notEqual">
+  <conditionalFormatting sqref="S22:V22">
+    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>$R22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" stopIfTrue="1" operator="equal">
       <formula>$R22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S3">
-    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="notEqual">
       <formula>$R2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" stopIfTrue="1" operator="equal">
       <formula>$R2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S27:U27">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="notEqual">
+  <conditionalFormatting sqref="S27:V27">
+    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>$R27</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="equal">
       <formula>$R27</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23:U23">
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="notEqual">
+  <conditionalFormatting sqref="S23:V23">
+    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>$R23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" stopIfTrue="1" operator="equal">
       <formula>$R23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:T28">
-    <cfRule type="cellIs" dxfId="5" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>$P8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="22" stopIfTrue="1" operator="equal">
       <formula>$P8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U25:U26">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="notEqual">
+      <formula>$R25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
+      <formula>$R25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U8:U28">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="notEqual">
+      <formula>$P8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" stopIfTrue="1" operator="equal">
+      <formula>$P8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V25:V26">
     <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>$R25</formula>
     </cfRule>
@@ -8315,7 +9109,7 @@
       <formula>$R25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U8:U28">
+  <conditionalFormatting sqref="V8:V28">
     <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>$P8</formula>
     </cfRule>

</xml_diff>